<commit_message>
Remove large files from the working directory
</commit_message>
<xml_diff>
--- a/Mapp_Differences.xlsx
+++ b/Mapp_Differences.xlsx
@@ -1642,6 +1642,45 @@
     <t>2024-02-18 15:08:05</t>
   </si>
   <si>
+    <t>PHZYMuYZy81kiB</t>
+  </si>
+  <si>
+    <t>[PHZYMuYZy81kiB PHTl2JAhUSu8s6 merchant PHZYM0x70Hkl2q 1730798554 1730798554 ]</t>
+  </si>
+  <si>
+    <t>1730798554</t>
+  </si>
+  <si>
+    <t>2024-11-05 14:52:34</t>
+  </si>
+  <si>
+    <t>ID not found in mapp_api.csv</t>
+  </si>
+  <si>
+    <t>P4YgZMYhoO9C6a</t>
+  </si>
+  <si>
+    <t>[P4YgZMYhoO9C6a C65yyS9pcolRUr referred P4YgYRvTyeMzWs 1727957076 1727957076 ]</t>
+  </si>
+  <si>
+    <t>1727957076</t>
+  </si>
+  <si>
+    <t>2024-10-03 17:34:36</t>
+  </si>
+  <si>
+    <t>P62kxToRP7l6xm</t>
+  </si>
+  <si>
+    <t>[P62kxToRP7l6xm C65yyS9pcolRUr referred P62kwFoO4o2awa 1728281314 1728281314 ]</t>
+  </si>
+  <si>
+    <t>1728281314</t>
+  </si>
+  <si>
+    <t>2024-10-07 11:38:34</t>
+  </si>
+  <si>
     <t>P4YjmZK5ukGRTR</t>
   </si>
   <si>
@@ -1654,7 +1693,28 @@
     <t>2024-10-03 17:37:39</t>
   </si>
   <si>
-    <t>ID not found in mapp_api.csv</t>
+    <t>PHZXGEvIsF1zmx</t>
+  </si>
+  <si>
+    <t>[PHZXGEvIsF1zmx PHWlZROPA0es90 merchant PHZXFL1AQ7fp1q 1730798491 1730798491 ]</t>
+  </si>
+  <si>
+    <t>1730798491</t>
+  </si>
+  <si>
+    <t>2024-11-05 14:51:31</t>
+  </si>
+  <si>
+    <t>PHZSWu73Wn9FkZ</t>
+  </si>
+  <si>
+    <t>[PHZSWu73Wn9FkZ PHZRkFuWQ2kKhs referred PHZSUvYf6ngG3k 1730798222 1730798222 ]</t>
+  </si>
+  <si>
+    <t>1730798222</t>
+  </si>
+  <si>
+    <t>2024-11-05 14:47:02</t>
   </si>
   <si>
     <t>P4rb4ZA28eywM3</t>
@@ -1667,66 +1727,6 @@
   </si>
   <si>
     <t>2024-10-04 12:04:35</t>
-  </si>
-  <si>
-    <t>PHZSWu73Wn9FkZ</t>
-  </si>
-  <si>
-    <t>[PHZSWu73Wn9FkZ PHZRkFuWQ2kKhs referred PHZSUvYf6ngG3k 1730798222 1730798222 ]</t>
-  </si>
-  <si>
-    <t>1730798222</t>
-  </si>
-  <si>
-    <t>2024-11-05 14:47:02</t>
-  </si>
-  <si>
-    <t>P62kxToRP7l6xm</t>
-  </si>
-  <si>
-    <t>[P62kxToRP7l6xm C65yyS9pcolRUr referred P62kwFoO4o2awa 1728281314 1728281314 ]</t>
-  </si>
-  <si>
-    <t>1728281314</t>
-  </si>
-  <si>
-    <t>2024-10-07 11:38:34</t>
-  </si>
-  <si>
-    <t>P4YgZMYhoO9C6a</t>
-  </si>
-  <si>
-    <t>[P4YgZMYhoO9C6a C65yyS9pcolRUr referred P4YgYRvTyeMzWs 1727957076 1727957076 ]</t>
-  </si>
-  <si>
-    <t>1727957076</t>
-  </si>
-  <si>
-    <t>2024-10-03 17:34:36</t>
-  </si>
-  <si>
-    <t>PHZYMuYZy81kiB</t>
-  </si>
-  <si>
-    <t>[PHZYMuYZy81kiB PHTl2JAhUSu8s6 merchant PHZYM0x70Hkl2q 1730798554 1730798554 ]</t>
-  </si>
-  <si>
-    <t>1730798554</t>
-  </si>
-  <si>
-    <t>2024-11-05 14:52:34</t>
-  </si>
-  <si>
-    <t>PHZXGEvIsF1zmx</t>
-  </si>
-  <si>
-    <t>[PHZXGEvIsF1zmx PHWlZROPA0es90 merchant PHZXFL1AQ7fp1q 1730798491 1730798491 ]</t>
-  </si>
-  <si>
-    <t>1730798491</t>
-  </si>
-  <si>
-    <t>2024-11-05 14:51:31</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Revert "Remove large files from the working directory"
This reverts commit f1f3d7f9d9e2c1714c03a4edc9c72184261a8467.
</commit_message>
<xml_diff>
--- a/Mapp_Differences.xlsx
+++ b/Mapp_Differences.xlsx
@@ -1642,6 +1642,69 @@
     <t>2024-02-18 15:08:05</t>
   </si>
   <si>
+    <t>P4YjmZK5ukGRTR</t>
+  </si>
+  <si>
+    <t>[P4YjmZK5ukGRTR C65yyS9pcolRUr referred P4YjleeSMz6H65 1727957259 1727957259 ]</t>
+  </si>
+  <si>
+    <t>1727957259</t>
+  </si>
+  <si>
+    <t>2024-10-03 17:37:39</t>
+  </si>
+  <si>
+    <t>ID not found in mapp_api.csv</t>
+  </si>
+  <si>
+    <t>P4rb4ZA28eywM3</t>
+  </si>
+  <si>
+    <t>[P4rb4ZA28eywM3 C65yyS9pcolRUr referred P4rb3LbPo3hd86 1728023675 1728023675 ]</t>
+  </si>
+  <si>
+    <t>1728023675</t>
+  </si>
+  <si>
+    <t>2024-10-04 12:04:35</t>
+  </si>
+  <si>
+    <t>PHZSWu73Wn9FkZ</t>
+  </si>
+  <si>
+    <t>[PHZSWu73Wn9FkZ PHZRkFuWQ2kKhs referred PHZSUvYf6ngG3k 1730798222 1730798222 ]</t>
+  </si>
+  <si>
+    <t>1730798222</t>
+  </si>
+  <si>
+    <t>2024-11-05 14:47:02</t>
+  </si>
+  <si>
+    <t>P62kxToRP7l6xm</t>
+  </si>
+  <si>
+    <t>[P62kxToRP7l6xm C65yyS9pcolRUr referred P62kwFoO4o2awa 1728281314 1728281314 ]</t>
+  </si>
+  <si>
+    <t>1728281314</t>
+  </si>
+  <si>
+    <t>2024-10-07 11:38:34</t>
+  </si>
+  <si>
+    <t>P4YgZMYhoO9C6a</t>
+  </si>
+  <si>
+    <t>[P4YgZMYhoO9C6a C65yyS9pcolRUr referred P4YgYRvTyeMzWs 1727957076 1727957076 ]</t>
+  </si>
+  <si>
+    <t>1727957076</t>
+  </si>
+  <si>
+    <t>2024-10-03 17:34:36</t>
+  </si>
+  <si>
     <t>PHZYMuYZy81kiB</t>
   </si>
   <si>
@@ -1654,45 +1717,6 @@
     <t>2024-11-05 14:52:34</t>
   </si>
   <si>
-    <t>ID not found in mapp_api.csv</t>
-  </si>
-  <si>
-    <t>P4YgZMYhoO9C6a</t>
-  </si>
-  <si>
-    <t>[P4YgZMYhoO9C6a C65yyS9pcolRUr referred P4YgYRvTyeMzWs 1727957076 1727957076 ]</t>
-  </si>
-  <si>
-    <t>1727957076</t>
-  </si>
-  <si>
-    <t>2024-10-03 17:34:36</t>
-  </si>
-  <si>
-    <t>P62kxToRP7l6xm</t>
-  </si>
-  <si>
-    <t>[P62kxToRP7l6xm C65yyS9pcolRUr referred P62kwFoO4o2awa 1728281314 1728281314 ]</t>
-  </si>
-  <si>
-    <t>1728281314</t>
-  </si>
-  <si>
-    <t>2024-10-07 11:38:34</t>
-  </si>
-  <si>
-    <t>P4YjmZK5ukGRTR</t>
-  </si>
-  <si>
-    <t>[P4YjmZK5ukGRTR C65yyS9pcolRUr referred P4YjleeSMz6H65 1727957259 1727957259 ]</t>
-  </si>
-  <si>
-    <t>1727957259</t>
-  </si>
-  <si>
-    <t>2024-10-03 17:37:39</t>
-  </si>
-  <si>
     <t>PHZXGEvIsF1zmx</t>
   </si>
   <si>
@@ -1703,30 +1727,6 @@
   </si>
   <si>
     <t>2024-11-05 14:51:31</t>
-  </si>
-  <si>
-    <t>PHZSWu73Wn9FkZ</t>
-  </si>
-  <si>
-    <t>[PHZSWu73Wn9FkZ PHZRkFuWQ2kKhs referred PHZSUvYf6ngG3k 1730798222 1730798222 ]</t>
-  </si>
-  <si>
-    <t>1730798222</t>
-  </si>
-  <si>
-    <t>2024-11-05 14:47:02</t>
-  </si>
-  <si>
-    <t>P4rb4ZA28eywM3</t>
-  </si>
-  <si>
-    <t>[P4rb4ZA28eywM3 C65yyS9pcolRUr referred P4rb3LbPo3hd86 1728023675 1728023675 ]</t>
-  </si>
-  <si>
-    <t>1728023675</t>
-  </si>
-  <si>
-    <t>2024-10-04 12:04:35</t>
   </si>
 </sst>
 </file>

</xml_diff>